<commit_message>
ajuste documento e importação
</commit_message>
<xml_diff>
--- a/tmp/uploads/Client_1/testeImportacao.xlsx
+++ b/tmp/uploads/Client_1/testeImportacao.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50BAC733-C6EE-4743-A17E-250AA715CE57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B37A07FC-8FA9-464E-A2A5-9C5C1874ADBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,35 +25,55 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Nome</t>
-  </si>
-  <si>
-    <t>Código</t>
-  </si>
-  <si>
-    <t>Livro</t>
-  </si>
-  <si>
-    <t>Folha</t>
-  </si>
-  <si>
-    <t>Bruno</t>
-  </si>
-  <si>
-    <t>Favato</t>
-  </si>
-  <si>
-    <t>Amaral</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>book</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>yeardoc</t>
+  </si>
+  <si>
+    <t>intfield1</t>
+  </si>
+  <si>
+    <t>stringfield1</t>
+  </si>
+  <si>
+    <t>datefield1</t>
+  </si>
+  <si>
+    <t>intfield2</t>
+  </si>
+  <si>
+    <t>stringfield2</t>
+  </si>
+  <si>
+    <t>datefield2</t>
+  </si>
+  <si>
+    <t>cod</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -81,8 +101,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -363,71 +389,603 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>59680</v>
+      </c>
+      <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1980</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>59681</v>
+      </c>
+      <c r="B3" s="1">
         <v>2</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1980</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>59682</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1980</v>
+      </c>
+      <c r="F4" s="1">
+        <v>3</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>59683</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1980</v>
+      </c>
+      <c r="F5" s="1">
+        <v>4</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>59684</v>
+      </c>
+      <c r="B6" s="1">
         <v>5</v>
       </c>
-      <c r="B3">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
         <v>2</v>
       </c>
-      <c r="C3">
+      <c r="E6" s="1">
+        <v>1980</v>
+      </c>
+      <c r="F6" s="1">
+        <v>5</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>59685</v>
+      </c>
+      <c r="B7" s="1">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
         <v>2</v>
       </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="E7" s="1">
+        <v>1980</v>
+      </c>
+      <c r="F7" s="1">
         <v>6</v>
       </c>
-      <c r="B4">
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>59686</v>
+      </c>
+      <c r="B8" s="1">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
         <v>3</v>
       </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
+      <c r="E8" s="1">
+        <v>1980</v>
+      </c>
+      <c r="F8" s="1">
+        <v>7</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>59687</v>
+      </c>
+      <c r="B9" s="1">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1">
         <v>3</v>
       </c>
+      <c r="E9" s="1">
+        <v>1980</v>
+      </c>
+      <c r="F9" s="1">
+        <v>8</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>59688</v>
+      </c>
+      <c r="B10" s="1">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1980</v>
+      </c>
+      <c r="F10" s="1">
+        <v>9</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>59689</v>
+      </c>
+      <c r="B11" s="1">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1">
+        <v>4</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1980</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>59690</v>
+      </c>
+      <c r="B12" s="1">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1">
+        <v>4</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1980</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>59691</v>
+      </c>
+      <c r="B13" s="1">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1">
+        <v>4</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1980</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>59692</v>
+      </c>
+      <c r="B14" s="1">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1">
+        <v>5</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1980</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>59693</v>
+      </c>
+      <c r="B15" s="1">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1">
+        <v>5</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1980</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1</v>
+      </c>
+      <c r="G15" s="1">
+        <v>1</v>
+      </c>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>59694</v>
+      </c>
+      <c r="B16" s="1">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1">
+        <v>5</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1980</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <v>1</v>
+      </c>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>59695</v>
+      </c>
+      <c r="B17" s="1">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1">
+        <v>6</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1980</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1">
+        <v>1</v>
+      </c>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>59696</v>
+      </c>
+      <c r="B18" s="1">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1">
+        <v>6</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1980</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1">
+        <v>1</v>
+      </c>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>59697</v>
+      </c>
+      <c r="B19" s="1">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1">
+        <v>6</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1980</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1</v>
+      </c>
+      <c r="G19" s="1">
+        <v>1</v>
+      </c>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>59698</v>
+      </c>
+      <c r="B20" s="1">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1">
+        <v>7</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1980</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1">
+        <v>1</v>
+      </c>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>59699</v>
+      </c>
+      <c r="B21" s="1">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1">
+        <v>7</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1980</v>
+      </c>
+      <c r="F21" s="1">
+        <v>1</v>
+      </c>
+      <c r="G21" s="1">
+        <v>1</v>
+      </c>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>